<commit_message>
All function has been added
</commit_message>
<xml_diff>
--- a/OnboardingTest2/OnboardingTest2/ExcelData/TestDataManageListings.xlsx
+++ b/OnboardingTest2/OnboardingTest2/ExcelData/TestDataManageListings.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Title</t>
   </si>
@@ -44,6 +44,12 @@
   </si>
   <si>
     <t>All kind of music lover</t>
+  </si>
+  <si>
+    <t>12.24.am</t>
+  </si>
+  <si>
+    <t>19.24.pm</t>
   </si>
 </sst>
 </file>
@@ -1086,16 +1092,16 @@
         <v>9</v>
       </c>
       <c r="D2" s="3">
-        <v>45052</v>
+        <v>45083</v>
       </c>
       <c r="E2" s="3">
         <v>45485</v>
       </c>
-      <c r="F2" s="4">
-        <v>12.24</v>
-      </c>
-      <c r="G2" s="4">
-        <v>19.24</v>
+      <c r="F2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>